<commit_message>
added Big decimal rates To calculate Frt Rates
added Big decimal rates
To calculate Frt Rates
</commit_message>
<xml_diff>
--- a/resources/RATES.xlsx
+++ b/resources/RATES.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="6435" windowWidth="16035" xWindow="600" yWindow="360"/>
+    <workbookView xWindow="600" yWindow="360" windowWidth="16035" windowHeight="6435"/>
   </bookViews>
   <sheets>
-    <sheet name="RATES" r:id="rId1" sheetId="1"/>
+    <sheet name="RATES" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Bill_Id</t>
   </si>
@@ -47,43 +47,12 @@
   </si>
   <si>
     <t>Total_Charge</t>
-  </si>
-  <si>
-    <t>15015.0</t>
-  </si>
-  <si>
-    <t>15016.0</t>
-  </si>
-  <si>
-    <t>15017.0</t>
-  </si>
-  <si>
-    <t>45014.0</t>
-  </si>
-  <si>
-    <t>45017.0</t>
-  </si>
-  <si>
-    <t>45018.0</t>
-  </si>
-  <si>
-    <t>45019.0</t>
-  </si>
-  <si>
-    <t>45020.0</t>
-  </si>
-  <si>
-    <t>45021.0</t>
-  </si>
-  <si>
-    <t>45022.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,98 +488,98 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="5" fontId="9" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="6" fontId="10" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="6" fontId="11" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="12" numFmtId="0"/>
-    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="7" fontId="13" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0"/>
-    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="8" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0"/>
-    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="16" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="17" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="17" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="19"/>
-    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="23"/>
-    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="27"/>
-    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="31"/>
-    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="35"/>
-    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="39"/>
-    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="20"/>
-    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="24"/>
-    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="28"/>
-    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="32"/>
-    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="36"/>
-    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="40"/>
-    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="21"/>
-    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="25"/>
-    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="29"/>
-    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="33"/>
-    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="37"/>
-    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="41"/>
-    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="18"/>
-    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="22"/>
-    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="26"/>
-    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="30"/>
-    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="34"/>
-    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="38"/>
-    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="7"/>
-    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="11"/>
-    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="13"/>
-    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="16"/>
-    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="6"/>
-    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="2"/>
-    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="3"/>
-    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="4"/>
-    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="5"/>
-    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="9"/>
-    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="12"/>
-    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="8"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="15"/>
-    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="10"/>
-    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="1"/>
-    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="17"/>
-    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="14"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -624,10 +593,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -785,7 +754,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -794,13 +763,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -810,7 +779,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -819,7 +788,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -828,7 +797,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -838,12 +807,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -874,7 +843,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -893,7 +862,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -905,14 +874,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -949,157 +921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>